<commit_message>
Add Header row setting. Edit version. Fix Error can raise.
</commit_message>
<xml_diff>
--- a/resources/data.xlsx
+++ b/resources/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d74986bd8fa84e9c/桌面/QRBatch/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pohan_lin\Desktop\QRBatch\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_F25DC773A252ABDACC104880819C48345ADE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABE6B08F-0959-4EF4-8C93-632D29F2413C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69C159F-EFF0-4DD4-A787-9F058F44822F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="3480" windowWidth="23040" windowHeight="8508" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7125" yWindow="1335" windowWidth="19410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,17 +104,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -150,7 +150,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -428,86 +428,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A2:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:9" ht="30">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="3" spans="1:9">
+      <c r="A3" s="1">
         <v>307</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>308</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -519,9 +493,35 @@
         <v>12</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1">
+        <v>308</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>